<commit_message>
Incoprorate dataref info in perf table
</commit_message>
<xml_diff>
--- a/tbmPerf.xlsx
+++ b/tbmPerf.xlsx
@@ -10,13 +10,14 @@
     <sheet name="MAXC" sheetId="1" r:id="rId1"/>
     <sheet name="NRMC" sheetId="2" r:id="rId2"/>
     <sheet name="LRC" sheetId="3" r:id="rId3"/>
+    <sheet name="TRQ" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Pressure Altitude</t>
   </si>
@@ -25,6 +26,12 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>pct</t>
+  </si>
+  <si>
+    <t>dref</t>
   </si>
 </sst>
 </file>
@@ -60,8 +67,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -74,6 +82,282 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TRQ!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dref</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:backward val="3"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1755676665282286E-2"/>
+                  <c:y val="-1.6981191304575299E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TRQ!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TRQ!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1966</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1032</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>879</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2434</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1179</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1390</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1581</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2229</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2529</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3033</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="157678208"/>
+        <c:axId val="157676672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="157678208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157676672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="157676672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157678208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,7 +650,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H19"/>
+      <selection activeCell="B3" sqref="B3:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,18 +1644,18 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5500</v>
+        <v>2495</v>
       </c>
       <c r="C2">
-        <v>6300</v>
+        <v>2858</v>
       </c>
       <c r="D2">
-        <v>7100</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="B3">
         <v>38</v>
@@ -1385,55 +1669,55 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5000</v>
+        <v>18000</v>
       </c>
       <c r="B4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>42</v>
       </c>
       <c r="D4">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10000</v>
+        <v>19000</v>
       </c>
       <c r="B5">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="B6">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="B7">
         <v>39</v>
       </c>
       <c r="C7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>49</v>
@@ -1441,13 +1725,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>19000</v>
+        <v>22000</v>
       </c>
       <c r="B8">
         <v>39</v>
       </c>
       <c r="C8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>49</v>
@@ -1455,13 +1739,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>20000</v>
+        <v>23000</v>
       </c>
       <c r="B9">
         <v>39</v>
       </c>
       <c r="C9">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>49</v>
@@ -1469,10 +1753,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="B10">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>44</v>
@@ -1483,10 +1767,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>22000</v>
+        <v>25000</v>
       </c>
       <c r="B11">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>44</v>
@@ -1497,131 +1781,322 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="B12">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C12">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C13">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>25000</v>
+        <v>28000</v>
       </c>
       <c r="B14">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C14">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D14">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>26000</v>
+        <v>29000</v>
       </c>
       <c r="B15">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D15">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>27000</v>
+        <v>30000</v>
       </c>
       <c r="B16">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D16">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>28000</v>
+        <v>31000</v>
       </c>
       <c r="B17">
         <v>46</v>
       </c>
       <c r="C17">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>29000</v>
-      </c>
-      <c r="B18">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>49</v>
-      </c>
-      <c r="D18">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>30000</v>
-      </c>
-      <c r="B19">
-        <v>46</v>
-      </c>
-      <c r="C19">
-        <v>50</v>
-      </c>
-      <c r="D19">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>31000</v>
-      </c>
-      <c r="B20">
-        <v>46</v>
-      </c>
-      <c r="C20">
-        <v>50</v>
-      </c>
-      <c r="D20">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>1444</v>
+      </c>
+      <c r="D2">
+        <f t="array" ref="D2:E6">LINEST(A2:A18,B2:B18, FALSE,TRUE)</f>
+        <v>3.3068537795767267E-2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f t="array" ref="F2:G6">LINEST(B2:B18,A2:A18,FALSE,TRUE)</f>
+        <v>30.238182501476405</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>1609</v>
+      </c>
+      <c r="D3">
+        <v>6.7933329969079839E-5</v>
+      </c>
+      <c r="E3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F3">
+        <v>6.2118876928419157E-2</v>
+      </c>
+      <c r="G3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>1722</v>
+      </c>
+      <c r="D4">
+        <v>0.99993248092538101</v>
+      </c>
+      <c r="E4">
+        <v>0.48559875222725246</v>
+      </c>
+      <c r="F4">
+        <v>0.99993248092538101</v>
+      </c>
+      <c r="G4">
+        <v>14.684119429782646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>59.8</v>
+      </c>
+      <c r="D5">
+        <v>236954.07238750803</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>236954.07238750989</v>
+      </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>1966</v>
+      </c>
+      <c r="D6">
+        <v>55875.227101629367</v>
+      </c>
+      <c r="E6">
+        <v>3.7728983706346328</v>
+      </c>
+      <c r="F6">
+        <v>51092834.066185147</v>
+      </c>
+      <c r="G6">
+        <v>3449.9738148499232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>879</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>100/D2</f>
+        <v>3024.0224293436972</v>
+      </c>
+      <c r="F8">
+        <f>F2*100</f>
+        <v>3023.8182501476404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>69</v>
+      </c>
+      <c r="B11">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>80</v>
+      </c>
+      <c r="B12">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>52</v>
+      </c>
+      <c r="B15">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>74</v>
+      </c>
+      <c r="B16">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>84</v>
+      </c>
+      <c r="B17">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>3033</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>